<commit_message>
Fixed microloan demisc fixesscription
</commit_message>
<xml_diff>
--- a/make_loan_info_json/LAT-loan-types.xlsx
+++ b/make_loan_info_json/LAT-loan-types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="145">
   <si>
     <t>loanID</t>
   </si>
@@ -344,6 +344,9 @@
     <t xml:space="preserve">Based on agency borrowing cost with a cap of 3.75%. View current rates </t>
   </si>
   <si>
+    <t xml:space="preserve">Rate based on agency borrowing cost with a cap of 3.75%. View current rates </t>
+  </si>
+  <si>
     <t>1-7 years for non-real-estate purposes. Up to 40 years for physical losses on real estate.</t>
   </si>
   <si>
@@ -441,6 +444,11 @@
   </si>
   <si>
     <t>https://lat.fpac.usda.gov/checklists/Youth%20Loan%20Readiness%20Checklist.pdf</t>
+  </si>
+  <si>
+    <t>Microloans are designed to fit the needs of small farms, beginning farmers, niche and non-traditional farm operations, to include truck farms, farms participating in direct marketing, such as farmers’ markets, CSAs (Community Supported Agriculture), restaurants, and grocery stores. Microloans can also be used for hydroponic, aquaponic, organic and vertical growing methods.|
+You may request up to $50,000 for a Operating Microloan and up to an additional $50,000 for an Microloan Farm Ownership. Note: The $50,000 limit includes any possible outstanding FSA Direct Operating or Farm Ownership unpaid principal loan balances.|
+A loan applicant may have a Guaranteed Operating Loan, Farm Ownership loan or Emergency Loan and still qualify for a Microloan. Need More Capital? Consider a Farm Ownership or Operating Loan.|</t>
   </si>
   <si>
     <t>https://lat.fpac.usda.gov/checklists/Microloan%20Readiness%20Checklist.pdf</t>
@@ -1008,9 +1016,7 @@
         <v>0.0</v>
       </c>
       <c r="X2" s="4"/>
-      <c r="Y2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
       <c r="AB2" s="9"/>
@@ -1535,16 +1541,18 @@
       <c r="Q9" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="R9" s="13"/>
+      <c r="R9" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="S9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U9" s="13"/>
       <c r="V9" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W9" s="8">
         <v>0.0</v>
@@ -1560,40 +1568,40 @@
         <v>4.0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N10" s="11">
         <v>5000.0</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="12" t="s">
@@ -1604,20 +1612,20 @@
         <v>37</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="W10" s="8">
         <v>0.0</v>
       </c>
       <c r="X10" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -1666,13 +1674,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
@@ -1699,16 +1707,16 @@
     </row>
     <row r="2" ht="56.25" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3">
@@ -7730,13 +7738,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>11</v>
@@ -7745,7 +7753,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
@@ -7775,13 +7783,13 @@
         <v>54</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>57</v>
@@ -7790,7 +7798,7 @@
         <v>58</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -7817,13 +7825,13 @@
         <v>71</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>73</v>
@@ -7835,7 +7843,7 @@
         <v>78</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -7876,7 +7884,7 @@
         <v>104</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -7900,24 +7908,24 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -7943,7 +7951,9 @@
       <c r="A6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="18" t="s">
+        <v>141</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="E6" s="25" t="s">
         <v>30</v>
@@ -7955,7 +7965,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7">
@@ -12026,7 +12036,7 @@
         <v>48</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>50</v>
@@ -12047,7 +12057,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
@@ -12068,7 +12078,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -12089,7 +12099,7 @@
         <v>71</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
@@ -12110,7 +12120,7 @@
         <v>71</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>50</v>
@@ -12131,7 +12141,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -12146,17 +12156,17 @@
         <v>4.0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G10" s="12"/>
     </row>

</xml_diff>

<commit_message>
Updated data in spreadsheet
</commit_message>
<xml_diff>
--- a/make_loan_info_json/LAT-loan-types.xlsx
+++ b/make_loan_info_json/LAT-loan-types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
   <si>
     <t>loanID</t>
   </si>
@@ -123,7 +123,7 @@
     <t>Operating Microloans are available up to a maximum of $50,000</t>
   </si>
   <si>
-    <t>View current rates</t>
+    <t>Based on agency borrowing cost. View current rates</t>
   </si>
   <si>
     <t>Rate based on agency borrowing cost.  View current rates</t>
@@ -161,10 +161,10 @@
     <t>Down payment loans made as microloans for farm ownership purposes may not exceed $50,000.</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>Farm Operating Loan</t>
+    <t>direct</t>
+  </si>
+  <si>
+    <t>Farm Ownership Loan</t>
   </si>
   <si>
     <t>FSA-2001, FSA-2002, FSA-2003, FSA-2004, FSA-2005, FSA-2006, FSA-2037, FSA-2038, FSA-2302</t>
@@ -174,66 +174,6 @@
   </si>
   <si>
     <t>FSA-2370, FSA-2150, FSA-2007, FSA-2014, FSA-2015, AD-3030</t>
-  </si>
-  <si>
-    <t>Annual Operating Loan</t>
-  </si>
-  <si>
-    <t>Used for regular operating expenses and repaid within 12 months or when the commodities produced are sold</t>
-  </si>
-  <si>
-    <t>FSA Farm Operating Loans may be used for normal operating expenses, machinery and equipment, minor real estate repairs or improvements, and refinancing debt. Operating Loans are a valuable resource to start, maintain and strengthen a farm or ranch. For new agricultural producers, Operating Loans provide an essential gateway into agricultural production by financing the cost of operating a farm. There are two types of Operating Loans to choose from, the main difference being the repayment terms. Annual operating loans are generally repaid within 12 months or when the commodities produced are sold. Term operating loans have a repayment period of up to 7 years.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Operating loans are not lines of credit and producers must reapply every year for an annual operating loan to continue the new year production cycle. </t>
-  </si>
-  <si>
-    <t>*Working with a commercial lender and interested in a Guarantee Operating Loan? Chat with your farm loan officer about this option.</t>
-  </si>
-  <si>
-    <t>term.jpg</t>
-  </si>
-  <si>
-    <t>A closeup on the face of a cow</t>
-  </si>
-  <si>
-    <t>$400,000 total between both Annual and Term Operating Loans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The direct loans are available up to a maximum of $400,000. </t>
-  </si>
-  <si>
-    <t>*FSA will guarantee farm operating loans through a commercial leader up to $2,037,000.</t>
-  </si>
-  <si>
-    <t>Based on agency borrowing cost. View current rates</t>
-  </si>
-  <si>
-    <t>12 months</t>
-  </si>
-  <si>
-    <t>*Or when the commodities produced are sold (no more than 18 months)</t>
-  </si>
-  <si>
-    <t>Annual operating loans are generally repaid within 12 months or when the commodities produced are sold.</t>
-  </si>
-  <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>Term Operating Loans</t>
-  </si>
-  <si>
-    <t>Used to purchase livestock, seed, and equipment. Loan funds can also cover startup costs and family living expenses</t>
-  </si>
-  <si>
-    <t>The repayment term may vary, but it cannot exceed seven years.</t>
-  </si>
-  <si>
-    <t>direct</t>
-  </si>
-  <si>
-    <t>Farm Ownership Loan</t>
   </si>
   <si>
     <t>Direct Farm Ownership Loan</t>
@@ -419,12 +359,24 @@
     <t>checklist</t>
   </si>
   <si>
+    <t>Farm Operating Loan</t>
+  </si>
+  <si>
+    <t>FSA Farm Operating Loans may be used for normal operating expenses, machinery and equipment, minor real estate repairs or improvements, and refinancing debt. Operating Loans are a valuable resource to start, maintain and strengthen a farm or ranch. For new agricultural producers, Operating Loans provide an essential gateway into agricultural production by financing the cost of operating a farm. There are two types of Operating Loans to choose from, the main difference being the repayment terms. Annual operating loans are generally repaid within 12 months or when the commodities produced are sold. Term operating loans have a repayment period of up to 7 years.</t>
+  </si>
+  <si>
     <t>Note: Operating loans are not lines of credit and producers must reapply every year for an annual operating loan to continue the new year production cycle.</t>
   </si>
   <si>
     <t>Used to fund regular operating expenses like purchase livestock, seed, and equipment. Loan funds can also cover startup costs and family living expenses</t>
   </si>
   <si>
+    <t>term.jpg</t>
+  </si>
+  <si>
+    <t>A closeup on the face of a cow</t>
+  </si>
+  <si>
     <t>https://lat.fpac.usda.gov/checklists/Annual%20and%20Term%20Operating%20Loan%20Readiness%20Checklist.pdf</t>
   </si>
   <si>
@@ -432,9 +384,6 @@
   </si>
   <si>
     <t>Note: Refinancing of real estate debt is not an authorized use of farm ownership loans.</t>
-  </si>
-  <si>
-    <t>Microloan Farm Ownership</t>
   </si>
   <si>
     <t>https://lat.fpac.usda.gov/checklists/Farm%20Ownership%20Loan%20Readiness%20Checklist.pdf</t>
@@ -454,7 +403,13 @@
     <t>https://lat.fpac.usda.gov/checklists/Microloan%20Readiness%20Checklist.pdf</t>
   </si>
   <si>
+    <t>annual</t>
+  </si>
+  <si>
     <t>FSA-2001</t>
+  </si>
+  <si>
+    <t>term</t>
   </si>
   <si>
     <t>FSA-2001, FSA-2309</t>
@@ -1106,73 +1061,29 @@
       <c r="AJ3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="8">
-        <v>0.0</v>
-      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="8"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="9"/>
@@ -1188,71 +1099,29 @@
       <c r="AJ4" s="10"/>
     </row>
     <row r="5">
-      <c r="A5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="12"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="W5" s="8">
-        <v>0.0</v>
-      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="8"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="9"/>
@@ -1272,10 +1141,10 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>49</v>
@@ -1287,57 +1156,57 @@
         <v>51</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="U6" s="13"/>
       <c r="V6" s="12" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="W6" s="8">
         <v>0.0</v>
       </c>
       <c r="X6" s="12" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="Z6" s="13"/>
       <c r="AA6" s="13"/>
@@ -1348,13 +1217,13 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
@@ -1363,57 +1232,57 @@
         <v>51</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="U7" s="13"/>
       <c r="V7" s="12" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="W7" s="14" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="X7" s="12" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
@@ -1424,13 +1293,13 @@
         <v>2.0</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>50</v>
@@ -1439,57 +1308,57 @@
         <v>51</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="K8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>96</v>
-      </c>
       <c r="P8" s="12" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="R8" s="13"/>
       <c r="S8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="U8" s="13"/>
       <c r="V8" s="12" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="W8" s="8">
         <v>0.0</v>
       </c>
       <c r="X8" s="12" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
@@ -1500,13 +1369,13 @@
         <v>3.0</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -1515,44 +1384,44 @@
         <v>51</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="N9" s="11">
         <v>500000.0</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="P9" s="13"/>
       <c r="Q9" s="12" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="U9" s="13"/>
       <c r="V9" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="W9" s="8">
         <v>0.0</v>
@@ -1568,64 +1437,64 @@
         <v>4.0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="N10" s="11">
         <v>5000.0</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="12" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="W10" s="8">
         <v>0.0</v>
       </c>
       <c r="X10" s="12" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -1641,15 +1510,13 @@
   <hyperlinks>
     <hyperlink r:id="rId1" ref="S2"/>
     <hyperlink r:id="rId2" ref="S3"/>
-    <hyperlink r:id="rId3" ref="S4"/>
-    <hyperlink r:id="rId4" ref="S5"/>
-    <hyperlink r:id="rId5" ref="S6"/>
-    <hyperlink r:id="rId6" ref="S7"/>
-    <hyperlink r:id="rId7" ref="S8"/>
-    <hyperlink r:id="rId8" ref="S9"/>
-    <hyperlink r:id="rId9" ref="S10"/>
+    <hyperlink r:id="rId3" ref="S6"/>
+    <hyperlink r:id="rId4" ref="S7"/>
+    <hyperlink r:id="rId5" ref="S8"/>
+    <hyperlink r:id="rId6" ref="S9"/>
+    <hyperlink r:id="rId7" ref="S10"/>
   </hyperlinks>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1674,13 +1541,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
@@ -1707,16 +1574,16 @@
     </row>
     <row r="2" ht="56.25" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
@@ -7738,13 +7605,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>11</v>
@@ -7753,7 +7620,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
@@ -7777,28 +7644,28 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -7822,28 +7689,28 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -7867,24 +7734,24 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -7908,24 +7775,24 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -7952,7 +7819,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5"/>
       <c r="E6" s="25" t="s">
@@ -7965,7 +7832,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
@@ -12030,13 +11897,13 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>50</v>
@@ -12051,13 +11918,13 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
@@ -12072,13 +11939,13 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -12093,13 +11960,13 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
@@ -12114,13 +11981,13 @@
         <v>2.0</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>50</v>
@@ -12135,13 +12002,13 @@
         <v>3.0</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -12156,17 +12023,17 @@
         <v>4.0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="G10" s="12"/>
     </row>

</xml_diff>